<commit_message>
Enhance MainWindow and ScheduleFrame functionality by adding window size configuration and import feature for Excel schedules. Implement fact collection in FactCollector to gather data from various sources, including weather and schedule activities. Update GeminiErrorCorrectionService to handle API key configuration via environment variables and improve suggestion generation based on collected facts. Refactor ScheduleController to read schedule data from Excel and save it to the database. Clean up imports and improve error handling across components.
</commit_message>
<xml_diff>
--- a/data/excel/thoi_khoa_bieu.xlsx
+++ b/data/excel/thoi_khoa_bieu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,129 +436,254 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Thứ 2</t>
+          <t>Thời gian</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Thứ 3</t>
+          <t>Thứ Hai</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Thứ 4</t>
+          <t>Thứ Ba</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Thứ 5</t>
+          <t>Thứ Tư</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Thứ 6</t>
+          <t>Thứ Năm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Thứ 7</t>
+          <t>Thứ Sáu</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Thứ Bảy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Chủ Nhật</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>06:00 – 08:00</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lập trình hướng đối tượng</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Trí tuệ nhân tạo</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Nguyên lý Hệ điều hành</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Tư tưởng HCM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Tiếng Anh 1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>(Đang đi làm)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Ôn tập nhanh tất cả môn (2h)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08:30 – 10:30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Trí tuệ nhân tạo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Nguyên lý HĐH</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Tư tưởng HCM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Tiếng Anh 1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Lập trình HĐTĐ</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>(Đang đi làm)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Hoàn thiện dự án nhỏ hàng tuần (2h)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>14:00 – 16:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nguyên lý Hệ điều hành</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tư tưởng HCM</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Tiếng Anh 1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Lập trình HĐTĐ</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Trí tuệ nhân tạo</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(Đang đi làm đến 17:00)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Buffer &amp; ôn chuyên sâu (2h)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>16:30 – 18:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tư tưởng HCM</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tiếng Anh 1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Lập trình HĐTĐ</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Trí tuệ nhân tạo</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Nguyên lý HĐH</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>17:00 – 18:30: Gym18:30 – 20:00: Ăn tối/ nghỉ</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nghỉ/nghỉ linh hoạt</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20:00 – 22:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Gym (tối)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gym (tối)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Gym (tối)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Gym (tối)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Gym (tối)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>20:00 – 22:00: Dự án nhỏ hàng tuần</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>20:00 – 21:30: Gym (tuỳ chọn)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update MainWindow title and enhance ScheduleFrame Excel import functionality with column mapping and validation checks. Log window size during startup for better debugging.
</commit_message>
<xml_diff>
--- a/data/excel/thoi_khoa_bieu.xlsx
+++ b/data/excel/thoi_khoa_bieu.xlsx
@@ -478,84 +478,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>06:00 – 08:00</t>
+          <t>06:00 – 07:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lập trình hướng đối tượng</t>
+          <t>OOP lý thuyết</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>DSA lý thuyết</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Nguyên lý Hệ điều hành</t>
+          <t>AI lý thuyết</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tư tưởng HCM</t>
+          <t>Bận lab</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Tiếng Anh 1</t>
+          <t>Tổng ôn DSA</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(Đang đi làm)</t>
+          <t>Tuỳ chọn AI/OOP</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Ôn tập nhanh tất cả môn (2h)</t>
+          <t>Ôn nhẹ + đọc thuật toán</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>08:30 – 10:30</t>
+          <t>08:00 – 10:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>AI thực hành</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Nguyên lý HĐH</t>
+          <t>DSA coding</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tư tưởng HCM</t>
+          <t>OOP code</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Tiếng Anh 1</t>
+          <t>Bận lab</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Lập trình HĐTĐ</t>
+          <t>AI mini-project</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(Đang đi làm)</t>
+          <t>Bận đi làm</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Hoàn thiện dự án nhỏ hàng tuần (2h)</t>
+          <t>Làm project AI</t>
         </is>
       </c>
     </row>
@@ -567,121 +567,121 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nguyên lý Hệ điều hành</t>
+          <t>OOP coding</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Tư tưởng HCM</t>
+          <t>AI lý thuyết</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tiếng Anh 1</t>
+          <t>DSA luyện tập</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lập trình HĐTĐ</t>
+          <t>Bận lab</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>Fix lỗi dự án</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(Đang đi làm đến 17:00)</t>
+          <t>Bận đi làm</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Buffer &amp; ôn chuyên sâu (2h)</t>
+          <t>Thi thử DSA / Leetcode</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:30 – 18:00</t>
+          <t>16:00 – 17:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tư tưởng HCM</t>
+          <t>Gym/cardio</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tiếng Anh 1</t>
+          <t>Gym/cardio</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Lập trình HĐTĐ</t>
+          <t>Gym/cardio</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Trí tuệ nhân tạo</t>
+          <t>Bận lab</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Nguyên lý HĐH</t>
+          <t>Gym/cardio</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>17:00 – 18:30: Gym18:30 – 20:00: Ăn tối/ nghỉ</t>
+          <t>Gym sau làm</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Nghỉ/nghỉ linh hoạt</t>
+          <t>Gym linh hoạt</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20:00 – 22:00</t>
+          <t>17:30 – 21:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gym (tối)</t>
+          <t>Bận</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gym (tối)</t>
+          <t>Bận</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Gym (tối)</t>
+          <t>Bận</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Gym (tối)</t>
+          <t>Bận</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Gym (tối)</t>
+          <t>Bận</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>20:00 – 22:00: Dự án nhỏ hàng tuần</t>
+          <t>Bận + gym</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>20:00 – 21:30: Gym (tuỳ chọn)</t>
+          <t>Bận / nghỉ ngơi</t>
         </is>
       </c>
     </row>

</xml_diff>